<commit_message>
-Adding some components to the design to improve the performance
</commit_message>
<xml_diff>
--- a/H17R10/Released/BOM/H17R10.xlsx
+++ b/H17R10/Released/BOM/H17R10.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H17R10\H17R10\release\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H17R10\H17R10\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A66F82-80ED-4BCD-9C2A-6F500BC5195A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D3A0BB-8621-4FA3-969D-894BF9F3FEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H21R00" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="158">
   <si>
     <t>Description</t>
   </si>
@@ -241,18 +241,6 @@
     <t>R1</t>
   </si>
   <si>
-    <t>Res 0.001 Ohm 1% 1W 2512</t>
-  </si>
-  <si>
-    <t>PR2512FKG070R001L</t>
-  </si>
-  <si>
-    <t>https://octopart.com/pr2512fkg070r001l-yageo-19033012?r=sp</t>
-  </si>
-  <si>
-    <t>R4 , R6</t>
-  </si>
-  <si>
     <t>R7, R8, R9, R10</t>
   </si>
   <si>
@@ -295,9 +283,6 @@
     <t>RES 39K OHM 1% 1/10W 0603</t>
   </si>
   <si>
-    <t>C1 ,C2, C4, C6, C8,C16, C17</t>
-  </si>
-  <si>
     <t>C11, C12, C13, C14</t>
   </si>
   <si>
@@ -430,9 +415,6 @@
     <t>ONSEMI</t>
   </si>
   <si>
-    <t>Rectifier Diode Small Signal Schottky 40V 0.3A 5ns 2-Pin SOD-323 T/R</t>
-  </si>
-  <si>
     <t>https://octopart.com/bat54slt1g-onsemi-21401?r=sp</t>
   </si>
   <si>
@@ -461,13 +443,70 @@
   </si>
   <si>
     <t>https://octopart.com/vlmy1300-gs08-vishay-21709204?r=sp</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>Res Thick Film 0603 1K Ohm 5% 1/10W ±100ppm/°C</t>
+  </si>
+  <si>
+    <t>RC0603JR-071KL</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rc0603jr-071kl-yageo-55402888?r=sp</t>
+  </si>
+  <si>
+    <t>PE2512FKE7W0R1L</t>
+  </si>
+  <si>
+    <t>RES 0.1 OHM 1% 2W 2512</t>
+  </si>
+  <si>
+    <t>https://octopart.com/pe2512fke7w0r1l-yageo-71384148?r=sp</t>
+  </si>
+  <si>
+    <t>C1 ,C2, C4, C6, C8,C16, C17,C22 ,C23</t>
+  </si>
+  <si>
+    <t>RES SMD 2K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>CRCW06032K00FKEA</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>https://octopart.com/crcw06032k00fkea-vishay-39455515?r=sp</t>
+  </si>
+  <si>
+    <t>R18</t>
+  </si>
+  <si>
+    <t>R17</t>
+  </si>
+  <si>
+    <t>RES SMD 100K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>CRCW0603100KFKEA</t>
+  </si>
+  <si>
+    <t>https://octopart.com/crcw0603100kfkea-vishay-39670900?r=sp</t>
+  </si>
+  <si>
+    <t>R4, R6, R19, R20, R21, R22</t>
+  </si>
+  <si>
+    <t>DIODE ARRAY SCHOTTKY 30V SOT23-3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -683,6 +722,12 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFFF0000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -1100,7 +1145,7 @@
     <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1152,6 +1197,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1173,25 +1227,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1610,9 +1646,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:G36"/>
+  <dimension ref="A2:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1656,11 +1694,11 @@
       <c r="C4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="22">
         <v>0</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1673,11 +1711,11 @@
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="20">
+      <c r="D5" s="23">
         <v>44893</v>
       </c>
-      <c r="E5" s="21"/>
-      <c r="F5" s="22"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="25"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1690,9 +1728,9 @@
       <c r="C6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="25"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="28"/>
       <c r="G6" s="2"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1755,21 +1793,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F11" s="16">
         <v>1</v>
@@ -1795,24 +1833,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="15" t="s">
-        <v>74</v>
+    <row r="13" spans="1:7" ht="24" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>156</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>71</v>
+        <v>144</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>73</v>
+        <v>145</v>
       </c>
       <c r="F13" s="16">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1837,299 +1875,299 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="27" t="s">
-        <v>80</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" s="36" t="s">
-        <v>83</v>
+      <c r="E15" s="21" t="s">
+        <v>79</v>
       </c>
       <c r="F15" s="16">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" s="17" t="s">
-        <v>62</v>
+      <c r="A16" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>140</v>
       </c>
       <c r="C16" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>42</v>
+        <v>141</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>142</v>
       </c>
       <c r="F16" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>147</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="F17" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="15" t="s">
+      <c r="C19" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="F17" s="16">
+      <c r="E19" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="16">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="F18" s="16">
+      <c r="C20" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="F20" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="C19" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="D19" s="15" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="E21" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="F21" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="36" t="s">
-        <v>103</v>
-      </c>
-      <c r="F19" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="B20" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="16">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="28" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="F21" s="16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>96</v>
+      <c r="E22" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="F22" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="36" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>109</v>
+        <v>146</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>110</v>
+        <v>64</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>106</v>
+        <v>30</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>107</v>
+        <v>15</v>
       </c>
       <c r="E23" s="18" t="s">
-        <v>108</v>
+        <v>31</v>
       </c>
       <c r="F23" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="24" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B24" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>34</v>
+        <v>85</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>89</v>
       </c>
       <c r="F24" s="16">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="B25" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25" s="16">
+      <c r="D26" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" s="35" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="F26" s="16">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="16">
         <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" s="32" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="C27" s="34" t="s">
-        <v>111</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="E27" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="F27" s="16">
-        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="E28" s="18" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="F28" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" s="33" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>123</v>
+        <v>86</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>125</v>
+        <v>95</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E29" s="18" t="s">
-        <v>126</v>
+        <v>94</v>
       </c>
       <c r="F29" s="16">
         <v>1</v>
@@ -2137,119 +2175,119 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C30" s="15" t="s">
-        <v>53</v>
+        <v>107</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>106</v>
       </c>
       <c r="D30" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>54</v>
+        <v>108</v>
+      </c>
+      <c r="E30" s="21" t="s">
+        <v>109</v>
       </c>
       <c r="F30" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="35" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>139</v>
+        <v>43</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>143</v>
+        <v>44</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>141</v>
+        <v>46</v>
       </c>
       <c r="D31" s="15" t="s">
-        <v>142</v>
+        <v>45</v>
       </c>
       <c r="E31" s="18" t="s">
-        <v>144</v>
+        <v>47</v>
       </c>
       <c r="F31" s="16">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="33" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="D32" s="15" t="s">
-        <v>133</v>
+        <v>20</v>
       </c>
       <c r="E32" s="18" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="F32" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="33" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F33" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A34" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D34" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="B33" s="15" t="s">
-        <v>137</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E33" s="18" t="s">
+      <c r="E34" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="F33" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E34" s="18" t="s">
-        <v>52</v>
-      </c>
       <c r="F34" s="16">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
-        <v>68</v>
+      <c r="A35" s="15" t="s">
+        <v>126</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>127</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>51</v>
+        <v>128</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F35" s="16">
         <v>1</v>
@@ -2257,21 +2295,81 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="D36" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="F36" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F37" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E38" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="F38" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B39" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C39" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D39" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E39" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="F36" s="16">
+      <c r="F39" s="16">
         <v>1</v>
       </c>
     </row>
@@ -2282,37 +2380,36 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E20" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E23" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="E9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E24" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E25" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E27" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E28" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="E12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E16" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E28" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E34" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E30" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="E36" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E18" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E31" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E37" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E33" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="E39" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="E14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="E10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E17" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E23" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E21" r:id="rId15" xr:uid="{B6A7E373-878E-4DC0-841F-5B7CE8889B0F}"/>
-    <hyperlink ref="E27" r:id="rId16" xr:uid="{3C36960E-4FBF-41B5-A695-EF587F7ADD8B}"/>
+    <hyperlink ref="E19" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E26" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E24" r:id="rId15" xr:uid="{B6A7E373-878E-4DC0-841F-5B7CE8889B0F}"/>
+    <hyperlink ref="E30" r:id="rId16" xr:uid="{3C36960E-4FBF-41B5-A695-EF587F7ADD8B}"/>
     <hyperlink ref="E15" r:id="rId17" xr:uid="{FDDA58BF-287C-45F8-9C73-A708B44448DE}"/>
-    <hyperlink ref="E19" r:id="rId18" xr:uid="{DCE3A79A-E87E-44CE-958A-B9EF75A65287}"/>
-    <hyperlink ref="E26" r:id="rId19" xr:uid="{4B391E39-BB20-43A8-8517-76544E79C451}"/>
-    <hyperlink ref="E29" r:id="rId20" xr:uid="{62272696-2D6B-4D3B-8662-6CC6093C6618}"/>
-    <hyperlink ref="E31" r:id="rId21" xr:uid="{2BBFEC54-C4E9-4F4C-9611-DA0E5282C6A7}"/>
-    <hyperlink ref="E32" r:id="rId22" xr:uid="{32538E4B-92D2-4BBA-93AF-C84E3FDDB292}"/>
-    <hyperlink ref="E33" r:id="rId23" xr:uid="{F9F3E152-BF93-4321-B0CA-7CF4B392CD72}"/>
-    <hyperlink ref="E35" r:id="rId24" xr:uid="{36A36A7E-93B6-40B6-A6B7-7521A1607BA1}"/>
+    <hyperlink ref="E22" r:id="rId18" xr:uid="{DCE3A79A-E87E-44CE-958A-B9EF75A65287}"/>
+    <hyperlink ref="E29" r:id="rId19" xr:uid="{4B391E39-BB20-43A8-8517-76544E79C451}"/>
+    <hyperlink ref="E32" r:id="rId20" xr:uid="{62272696-2D6B-4D3B-8662-6CC6093C6618}"/>
+    <hyperlink ref="E34" r:id="rId21" xr:uid="{2BBFEC54-C4E9-4F4C-9611-DA0E5282C6A7}"/>
+    <hyperlink ref="E35" r:id="rId22" xr:uid="{32538E4B-92D2-4BBA-93AF-C84E3FDDB292}"/>
+    <hyperlink ref="E36" r:id="rId23" xr:uid="{F9F3E152-BF93-4321-B0CA-7CF4B392CD72}"/>
+    <hyperlink ref="E38" r:id="rId24" xr:uid="{36A36A7E-93B6-40B6-A6B7-7521A1607BA1}"/>
     <hyperlink ref="E11" r:id="rId25" xr:uid="{C51BD8F0-ECD4-45A4-B78A-1B3EBA1A640E}"/>
-    <hyperlink ref="E13" r:id="rId26" xr:uid="{8AE15586-36C9-49B0-B82C-DAED02694075}"/>
-    <hyperlink ref="E18" r:id="rId27" xr:uid="{E15B574F-CABD-4497-ADCC-48B492161F95}"/>
-    <hyperlink ref="E22" r:id="rId28" xr:uid="{DF4F0062-9A6F-43B4-8E79-8D484D752EB4}"/>
+    <hyperlink ref="E20" r:id="rId26" xr:uid="{E15B574F-CABD-4497-ADCC-48B492161F95}"/>
+    <hyperlink ref="E25" r:id="rId27" xr:uid="{DF4F0062-9A6F-43B4-8E79-8D484D752EB4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId29"/>
-  <drawing r:id="rId30"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId28"/>
+  <drawing r:id="rId29"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
-Connect missing wires - Delete power led - Improve the layout for better performance and appearance
</commit_message>
<xml_diff>
--- a/H17R10/Released/BOM/H17R10.xlsx
+++ b/H17R10/Released/BOM/H17R10.xlsx
@@ -5,27 +5,37 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\OneDrive\Documents\H17R1x-Hardware\H17R10\Released\BOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HEXABITZ\Modules\Hardware\Modules Hardware Design\H17R10\Corrected_Virsion\H17R10\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAD802B-4559-4123-97F0-8ED721ECFA28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D8C36A-2B55-4545-9B83-6D8ED3284AED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H17R10" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="158">
   <si>
     <t>Description</t>
   </si>
@@ -91,9 +101,6 @@
     <t>Vishay</t>
   </si>
   <si>
-    <t>JP1</t>
-  </si>
-  <si>
     <t>PCB Header, Unshrouded, Thru 02 Straight Header, .101, AMPMODU Mod II Series</t>
   </si>
   <si>
@@ -106,9 +113,6 @@
     <t>https://octopart.com/87227-1-te+connectivity-39512052?r=sp</t>
   </si>
   <si>
-    <t>JP2</t>
-  </si>
-  <si>
     <t>Conn Unshrouded Header HDR 3 POS 2.54mm Solder ST Top Entry Thru-Hole Carton</t>
   </si>
   <si>
@@ -250,9 +254,6 @@
     <t>https://octopart.com/rc0805fr-0710kl-yageo-40301103?r=sp</t>
   </si>
   <si>
-    <t>R11, R12, R15</t>
-  </si>
-  <si>
     <t>RES 10K OHM 1% 1/8W 0805</t>
   </si>
   <si>
@@ -367,9 +368,6 @@
     <t>C19</t>
   </si>
   <si>
-    <t>J1</t>
-  </si>
-  <si>
     <t>M20-9990245</t>
   </si>
   <si>
@@ -382,18 +380,6 @@
     <t>https://octopart.com/m20-9990245-harwin-7492269?r=sp</t>
   </si>
   <si>
-    <t>D9</t>
-  </si>
-  <si>
-    <t>VLMTG1300-GS08</t>
-  </si>
-  <si>
-    <t>LED Uni-Color True Green 530nm 2-Pin Chip 0603(1608Metric) T/R</t>
-  </si>
-  <si>
-    <t>https://octopart.com/vlmtg1300-gs08-vishay-21709202?r=sp</t>
-  </si>
-  <si>
     <t>POWERSTEP01</t>
   </si>
   <si>
@@ -500,17 +486,41 @@
   </si>
   <si>
     <t>DIODE ARRAY SCHOTTKY 30V SOT23-3</t>
+  </si>
+  <si>
+    <t>A, B, PWR</t>
+  </si>
+  <si>
+    <t>Block, Terminal; 13.5 A; 250 V; 5 mm; 26 to 16 AWG; 2; Screw; Solder; 4 kV; PA</t>
+  </si>
+  <si>
+    <t>Phoenix Contact</t>
+  </si>
+  <si>
+    <t>https://octopart.com/1729018-phoenix+contact-8551?r=sp</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>SWD</t>
+  </si>
+  <si>
+    <t>EMG_SW</t>
+  </si>
+  <si>
+    <t>R11, R15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -518,7 +528,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -529,21 +539,21 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -556,7 +566,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -577,7 +587,7 @@
     <font>
       <b/>
       <sz val="36"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -596,14 +606,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -611,7 +621,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -619,7 +629,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -627,28 +637,28 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -656,7 +666,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -664,14 +674,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -679,14 +689,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -694,7 +704,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -702,21 +712,21 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -725,8 +735,16 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -910,6 +928,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1139,7 +1163,7 @@
     <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1197,8 +1221,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1220,6 +1244,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1299,7 +1326,7 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>2174599</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:rowOff>20002</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1639,22 +1666,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="70.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.69921875" customWidth="1"/>
+    <col min="2" max="2" width="70.59765625" customWidth="1"/>
+    <col min="3" max="3" width="21.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.8984375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="84" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.3984375" customWidth="1"/>
     <col min="7" max="7" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" ht="46.2" x14ac:dyDescent="0.85">
+    <row r="2" spans="1:7" ht="45.6" x14ac:dyDescent="0.75">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
       <c r="C2" s="9" t="s">
@@ -1666,7 +1693,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1675,7 +1702,7 @@
       <c r="F3" s="11"/>
       <c r="G3" s="12"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>7</v>
       </c>
@@ -1692,29 +1719,29 @@
       <c r="F4" s="22"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="23">
-        <v>44893</v>
+        <v>45055</v>
       </c>
       <c r="E5" s="24"/>
       <c r="F5" s="25"/>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>14</v>
@@ -1724,7 +1751,7 @@
       <c r="F6" s="28"/>
       <c r="G6" s="2"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1744,621 +1771,621 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1729018</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="F9" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="C10" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="E10" s="18" t="s">
         <v>24</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>29</v>
       </c>
       <c r="F10" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>113</v>
+        <v>155</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>116</v>
+        <v>25</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>114</v>
+        <v>26</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>115</v>
+        <v>22</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>117</v>
+        <v>27</v>
       </c>
       <c r="F11" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>70</v>
+        <v>156</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>35</v>
+        <v>112</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>37</v>
+        <v>110</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="F12" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
-        <v>156</v>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>144</v>
+        <v>33</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>143</v>
+        <v>35</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>78</v>
+        <v>34</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>145</v>
+        <v>36</v>
       </c>
       <c r="F13" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="F14" s="16">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="17" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="E14" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" s="16">
+      <c r="E15" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B16" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="D16" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="F15" s="16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>140</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>142</v>
-      </c>
       <c r="F16" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>147</v>
+        <v>131</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>132</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>149</v>
+        <v>34</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="F17" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="17" t="s">
-        <v>62</v>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>139</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>42</v>
+        <v>140</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>142</v>
       </c>
       <c r="F18" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" s="16">
+      <c r="F20" s="16">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="15" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="F20" s="16">
+      <c r="F21" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>153</v>
-      </c>
-      <c r="C21" s="15" t="s">
-        <v>154</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>155</v>
-      </c>
-      <c r="F21" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>97</v>
+        <v>144</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>146</v>
       </c>
       <c r="D22" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>98</v>
+        <v>141</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>147</v>
       </c>
       <c r="F22" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="39.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
-        <v>146</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>64</v>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>96</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="D23" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="18" t="s">
-        <v>31</v>
+      <c r="E23" s="20" t="s">
+        <v>95</v>
       </c>
       <c r="F23" s="16">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>85</v>
+        <v>138</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>88</v>
+        <v>28</v>
       </c>
       <c r="D24" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="E24" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="F25" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="F24" s="16">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="B25" s="15" t="s">
+      <c r="C26" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="F26" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="F27" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="B30" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C30" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="D25" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="E25" s="18" t="s">
+      <c r="D30" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="F25" s="16">
+      <c r="F30" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="15" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B31" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="C31" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C26" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="F26" s="16">
+      <c r="E31" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="F27" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="F29" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="C30" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="F30" s="16">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="15" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C31" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="15" t="s">
+      <c r="E32" s="18" t="s">
         <v>45</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="F31" s="16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" s="18" t="s">
-        <v>121</v>
       </c>
       <c r="F32" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D33" s="15" t="s">
         <v>20</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F33" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D34" s="15" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E34" s="18" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="F34" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="D35" s="15" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="E35" s="18" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="F35" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E36" s="18" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="F36" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="E37" s="18" t="s">
         <v>50</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D37" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E37" s="18" t="s">
-        <v>52</v>
       </c>
       <c r="F37" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E38" s="18" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="F38" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" s="15" t="s">
         <v>55</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>57</v>
       </c>
       <c r="D39" s="15" t="s">
         <v>16</v>
       </c>
       <c r="E39" s="18" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F39" s="16">
         <v>1</v>
@@ -2371,36 +2398,35 @@
     <mergeCell ref="D6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="E23" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E27" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E28" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E18" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E31" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E24" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E10" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E28" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E29" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E13" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E19" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E32" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="E37" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
     <hyperlink ref="E33" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="E39" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E19" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E26" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E24" r:id="rId15" xr:uid="{B6A7E373-878E-4DC0-841F-5B7CE8889B0F}"/>
-    <hyperlink ref="E30" r:id="rId16" xr:uid="{3C36960E-4FBF-41B5-A695-EF587F7ADD8B}"/>
-    <hyperlink ref="E15" r:id="rId17" xr:uid="{FDDA58BF-287C-45F8-9C73-A708B44448DE}"/>
-    <hyperlink ref="E22" r:id="rId18" xr:uid="{DCE3A79A-E87E-44CE-958A-B9EF75A65287}"/>
-    <hyperlink ref="E29" r:id="rId19" xr:uid="{4B391E39-BB20-43A8-8517-76544E79C451}"/>
-    <hyperlink ref="E32" r:id="rId20" xr:uid="{62272696-2D6B-4D3B-8662-6CC6093C6618}"/>
-    <hyperlink ref="E34" r:id="rId21" xr:uid="{2BBFEC54-C4E9-4F4C-9611-DA0E5282C6A7}"/>
-    <hyperlink ref="E35" r:id="rId22" xr:uid="{32538E4B-92D2-4BBA-93AF-C84E3FDDB292}"/>
-    <hyperlink ref="E36" r:id="rId23" xr:uid="{F9F3E152-BF93-4321-B0CA-7CF4B392CD72}"/>
-    <hyperlink ref="E38" r:id="rId24" xr:uid="{36A36A7E-93B6-40B6-A6B7-7521A1607BA1}"/>
-    <hyperlink ref="E11" r:id="rId25" xr:uid="{C51BD8F0-ECD4-45A4-B78A-1B3EBA1A640E}"/>
-    <hyperlink ref="E20" r:id="rId26" xr:uid="{E15B574F-CABD-4497-ADCC-48B492161F95}"/>
-    <hyperlink ref="E25" r:id="rId27" xr:uid="{DF4F0062-9A6F-43B4-8E79-8D484D752EB4}"/>
+    <hyperlink ref="E15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="E11" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E20" r:id="rId13" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E27" r:id="rId14" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E25" r:id="rId15" xr:uid="{B6A7E373-878E-4DC0-841F-5B7CE8889B0F}"/>
+    <hyperlink ref="E31" r:id="rId16" xr:uid="{3C36960E-4FBF-41B5-A695-EF587F7ADD8B}"/>
+    <hyperlink ref="E16" r:id="rId17" xr:uid="{FDDA58BF-287C-45F8-9C73-A708B44448DE}"/>
+    <hyperlink ref="E23" r:id="rId18" xr:uid="{DCE3A79A-E87E-44CE-958A-B9EF75A65287}"/>
+    <hyperlink ref="E30" r:id="rId19" xr:uid="{4B391E39-BB20-43A8-8517-76544E79C451}"/>
+    <hyperlink ref="E34" r:id="rId20" xr:uid="{2BBFEC54-C4E9-4F4C-9611-DA0E5282C6A7}"/>
+    <hyperlink ref="E35" r:id="rId21" xr:uid="{32538E4B-92D2-4BBA-93AF-C84E3FDDB292}"/>
+    <hyperlink ref="E36" r:id="rId22" xr:uid="{F9F3E152-BF93-4321-B0CA-7CF4B392CD72}"/>
+    <hyperlink ref="E38" r:id="rId23" xr:uid="{36A36A7E-93B6-40B6-A6B7-7521A1607BA1}"/>
+    <hyperlink ref="E12" r:id="rId24" xr:uid="{C51BD8F0-ECD4-45A4-B78A-1B3EBA1A640E}"/>
+    <hyperlink ref="E21" r:id="rId25" xr:uid="{E15B574F-CABD-4497-ADCC-48B492161F95}"/>
+    <hyperlink ref="E26" r:id="rId26" xr:uid="{DF4F0062-9A6F-43B4-8E79-8D484D752EB4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId28"/>
-  <drawing r:id="rId29"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId27"/>
+  <drawing r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>